<commit_message>
Completed tasks 2 and 3
</commit_message>
<xml_diff>
--- a/misc/Part_2_and_3.xlsx
+++ b/misc/Part_2_and_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wind3\Documents\course\takehome\dbt_takehomeproject\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C5B7E2-ED89-4869-A2D3-3C859FBD8DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4982833C-5B80-41F3-BBEC-6C1A02BD51B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{5C8046D4-B854-4770-B099-3FB16B6A87B4}"/>
   </bookViews>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>So that…</t>
-  </si>
-  <si>
-    <t>US No.</t>
   </si>
   <si>
     <t>As a Product Manager</t>
@@ -229,21 +226,6 @@
     <t>Workshop to define Business Rules</t>
   </si>
   <si>
-    <t>Create Synthetic Test Cases</t>
-  </si>
-  <si>
-    <t>Build Isolated Prototypes</t>
-  </si>
-  <si>
-    <t>Share Results with Business Users</t>
-  </si>
-  <si>
-    <t>Iterate Based on Feedback</t>
-  </si>
-  <si>
-    <t>Bake into Production Metric</t>
-  </si>
-  <si>
     <t>Power BI/Tableau dashboard or Excel</t>
   </si>
   <si>
@@ -268,9 +250,6 @@
     <t>Valid Dates Check</t>
   </si>
   <si>
-    <t>Policy start date must be before end date.</t>
-  </si>
-  <si>
     <t>Prevents negative or zero-day lifetimes.</t>
   </si>
   <si>
@@ -283,9 +262,6 @@
     <t>Ensures policies aren't falsely stitched together across long gaps.</t>
   </si>
   <si>
-    <t>Policies should not go from "Cancelled" to "Active" without a valid reinstatement.</t>
-  </si>
-  <si>
     <t>WHERE prev_status = 'Cancelled' AND current_status = 'Active' AND reinstated_flag = FALSE</t>
   </si>
   <si>
@@ -298,22 +274,46 @@
     <t>Business Rule</t>
   </si>
   <si>
-    <t>WHERE policy_start_date &gt;= policy_end_date</t>
-  </si>
-  <si>
     <t>Use-case</t>
   </si>
   <si>
-    <t>If a policy is reinstated, the reinstatement date must be ≤ gap window (ex., 30 days after cancellation).</t>
-  </si>
-  <si>
     <t>Create small sample datasets that simulate each edge case (ex., a policy that is reinstated after 20 days)</t>
   </si>
   <si>
-    <t>Meet with the stakeholders to confirm the business logic for each edge case (ex., “reinstatement = within 30 days?” otherwise cancel the policy?, "what happens if payment is more than 30 days from due date?")</t>
-  </si>
-  <si>
     <t>Consistent Status Transitions with reinstatement flag</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Meet with the stakeholders to confirm the business logic for each edge case (ex., “reinstatement = within 30 days?”, "what happens if payment is more than 30 days from due date?")</t>
+  </si>
+  <si>
+    <t>Test data set-up / Create Synthetic Test Cases</t>
+  </si>
+  <si>
+    <t>Policies should not go from "Cancelled" to "Active" without a valid reinstatement</t>
+  </si>
+  <si>
+    <t>Policy start date must be before end date and there are no missing or null values</t>
+  </si>
+  <si>
+    <t>WHERE policy_start_date &gt;= policy_end_date AND (policy_start_date is NULL OR policy_end_date is NULL)</t>
+  </si>
+  <si>
+    <t>If a policy is reinstated, the reinstatement date must be less than or equal to grace period (ex., 30 days after cancellation)</t>
+  </si>
+  <si>
+    <t>Iterate based on feedback</t>
+  </si>
+  <si>
+    <t>Share results with business users</t>
+  </si>
+  <si>
+    <t>Build prototypes</t>
+  </si>
+  <si>
+    <t>Bake into production metric</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -558,18 +558,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -578,19 +575,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -598,15 +592,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -620,24 +605,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -957,7 +942,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -970,33 +955,33 @@
     <col min="6" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="41" t="s">
+      <c r="A2" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="32" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1005,19 +990,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1038,11 +1023,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D154FC05-7201-4F79-B93D-55D3550624B2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1053,58 +1038,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.8">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.8">
-      <c r="A2" s="12">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8">
-      <c r="A3" s="12">
-        <v>2</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="14" t="s">
+    <row r="4" spans="1:3" ht="29.4" thickBot="1">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="29.4" thickBot="1">
-      <c r="A4" s="15">
-        <v>3</v>
-      </c>
-      <c r="B4" s="16" t="s">
+      <c r="C4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1116,7 +1091,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.109375" defaultRowHeight="14.4"/>
@@ -1128,109 +1103,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.2">
+      <c r="A3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="57.6">
-      <c r="A3" s="22" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="28.8">
+      <c r="A4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8">
+      <c r="A5" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8">
+      <c r="A6" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.8">
-      <c r="A4" s="22" t="s">
+      <c r="D6" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8">
+      <c r="A7" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8">
-      <c r="A5" s="22" t="s">
+      <c r="C7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29.4" thickBot="1">
+      <c r="A8" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>38</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8">
-      <c r="A6" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8">
-      <c r="A7" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29.4" thickBot="1">
-      <c r="A8" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1246,65 +1221,65 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.44140625" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="52.8">
+      <c r="A2" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="57.6">
+      <c r="A3" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.2">
+      <c r="A4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="C4" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8">
-      <c r="A2" s="20" t="s">
+      <c r="D4" s="16" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="57.6">
-      <c r="A3" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.2">
-      <c r="A4" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>